<commit_message>
Cambios en escaleta y guion LE_06_08_CO
Se incluyó un recurso que había quedado por fuera
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion08/ESCALETA_LE_06_08_CO_VERSION2.xlsx
+++ b/fuentes/contenidos/grado06/guion08/ESCALETA_LE_06_08_CO_VERSION2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="289">
   <si>
     <t>Asignatura</t>
   </si>
@@ -899,6 +899,21 @@
   </si>
   <si>
     <t>LE_06_08_CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La organización de un sociodrama </t>
+  </si>
+  <si>
+    <t>Los roles en un sociodrama</t>
+  </si>
+  <si>
+    <t>Actividad sobre tareas y funciones de los participantes en sociodramas</t>
+  </si>
+  <si>
+    <t>Establecer algunos roles de los participantes en sociodramas y sus características o funciones, para que el estudiante los organice.</t>
+  </si>
+  <si>
+    <t>Recurso M10A-03</t>
   </si>
 </sst>
 </file>
@@ -1185,16 +1200,34 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1240,24 +1273,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1566,9 +1581,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,94 +1612,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="K1" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="47"/>
-      <c r="O1" s="35" t="s">
+      <c r="N1" s="53"/>
+      <c r="O1" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="R1" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="54" t="s">
+      <c r="T1" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="U1" s="35" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="42"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="48"/>
       <c r="M2" s="26" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="53"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="36"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -2784,49 +2799,51 @@
         <v>142</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>151</v>
+        <v>284</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="16" t="s">
-        <v>232</v>
+        <v>285</v>
       </c>
       <c r="H21" s="9">
         <v>19</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>233</v>
+        <v>286</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
+      <c r="N21" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="O21" s="9" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="P21" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q21" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>159</v>
+        <v>288</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2843,51 +2860,49 @@
         <v>142</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="16" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="H22" s="9">
         <v>20</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M22" s="8"/>
-      <c r="N22" s="8" t="s">
-        <v>121</v>
-      </c>
+      <c r="N22" s="8"/>
       <c r="O22" s="9" t="s">
-        <v>239</v>
+        <v>280</v>
       </c>
       <c r="P22" s="9" t="s">
         <v>19</v>
       </c>
       <c r="Q22" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>240</v>
+        <v>159</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2901,34 +2916,36 @@
         <v>138</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="E23" s="13"/>
+        <v>142</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>123</v>
+      </c>
       <c r="F23" s="9"/>
       <c r="G23" s="16" t="s">
-        <v>246</v>
+        <v>227</v>
       </c>
       <c r="H23" s="9">
         <v>21</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="N23" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="O23" s="9" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="P23" s="9" t="s">
         <v>19</v>
@@ -2937,16 +2954,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>192</v>
+        <v>129</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>193</v>
+        <v>130</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>195</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -2962,12 +2979,10 @@
       <c r="D24" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>153</v>
-      </c>
+      <c r="E24" s="13"/>
       <c r="F24" s="9"/>
       <c r="G24" s="16" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H24" s="9">
         <v>22</v>
@@ -2976,7 +2991,7 @@
         <v>19</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
@@ -2985,11 +3000,11 @@
         <v>5</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N24" s="8"/>
       <c r="O24" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="P24" s="9" t="s">
         <v>19</v>
@@ -3004,7 +3019,7 @@
         <v>193</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="U24" s="10" t="s">
         <v>195</v>
@@ -3024,33 +3039,33 @@
         <v>144</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="16" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="H25" s="9">
         <v>23</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8" t="s">
-        <v>121</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N25" s="8"/>
       <c r="O25" s="9" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="P25" s="9" t="s">
         <v>19</v>
@@ -3059,16 +3074,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="11" t="s">
-        <v>129</v>
+        <v>192</v>
       </c>
       <c r="S25" s="10" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="T25" s="12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>131</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3082,36 +3097,36 @@
         <v>138</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="16" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
       <c r="H26" s="9">
         <v>24</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="N26" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="O26" s="9" t="s">
-        <v>282</v>
+        <v>255</v>
       </c>
       <c r="P26" s="9" t="s">
         <v>19</v>
@@ -3120,16 +3135,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="11" t="s">
-        <v>192</v>
+        <v>129</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>193</v>
+        <v>130</v>
       </c>
       <c r="T26" s="12" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>195</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3146,33 +3161,33 @@
         <v>143</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="16" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="H27" s="9">
         <v>25</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8" t="s">
-        <v>121</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" s="8"/>
       <c r="O27" s="9" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="P27" s="9" t="s">
         <v>19</v>
@@ -3184,13 +3199,13 @@
         <v>192</v>
       </c>
       <c r="S27" s="10" t="s">
-        <v>264</v>
+        <v>193</v>
       </c>
       <c r="T27" s="12" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="U27" s="10" t="s">
-        <v>266</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3211,7 +3226,7 @@
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H28" s="9">
         <v>26</v>
@@ -3220,7 +3235,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>20</v>
@@ -3230,28 +3245,28 @@
       </c>
       <c r="M28" s="8"/>
       <c r="N28" s="8" t="s">
-        <v>36</v>
+        <v>121</v>
       </c>
       <c r="O28" s="9" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q28" s="10">
         <v>6</v>
       </c>
       <c r="R28" s="11" t="s">
-        <v>129</v>
+        <v>192</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>130</v>
+        <v>264</v>
       </c>
       <c r="T28" s="12" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>131</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3265,12 +3280,14 @@
         <v>138</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="E29" s="13"/>
+        <v>143</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="F29" s="9"/>
       <c r="G29" s="16" t="s">
-        <v>212</v>
+        <v>271</v>
       </c>
       <c r="H29" s="9">
         <v>27</v>
@@ -3279,7 +3296,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>213</v>
+        <v>272</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>20</v>
@@ -3289,13 +3306,13 @@
       </c>
       <c r="M29" s="8"/>
       <c r="N29" s="8" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>214</v>
+        <v>273</v>
       </c>
       <c r="P29" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q29" s="10">
         <v>6</v>
@@ -3307,7 +3324,7 @@
         <v>130</v>
       </c>
       <c r="T29" s="12" t="s">
-        <v>215</v>
+        <v>274</v>
       </c>
       <c r="U29" s="10" t="s">
         <v>131</v>
@@ -3329,7 +3346,7 @@
       <c r="E30" s="13"/>
       <c r="F30" s="9"/>
       <c r="G30" s="16" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
       <c r="H30" s="9">
         <v>28</v>
@@ -3338,7 +3355,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="17" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
       <c r="K30" s="7" t="s">
         <v>20</v>
@@ -3348,10 +3365,10 @@
       </c>
       <c r="M30" s="8"/>
       <c r="N30" s="8" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>243</v>
+        <v>214</v>
       </c>
       <c r="P30" s="9" t="s">
         <v>19</v>
@@ -3366,7 +3383,7 @@
         <v>130</v>
       </c>
       <c r="T30" s="12" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
       <c r="U30" s="10" t="s">
         <v>131</v>
@@ -3388,7 +3405,7 @@
       <c r="E31" s="13"/>
       <c r="F31" s="9"/>
       <c r="G31" s="16" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="H31" s="9">
         <v>29</v>
@@ -3397,7 +3414,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="17" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>20</v>
@@ -3407,10 +3424,10 @@
       </c>
       <c r="M31" s="8"/>
       <c r="N31" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="P31" s="9" t="s">
         <v>19</v>
@@ -3425,7 +3442,7 @@
         <v>130</v>
       </c>
       <c r="T31" s="12" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="U31" s="10" t="s">
         <v>131</v>
@@ -3447,7 +3464,7 @@
       <c r="E32" s="13"/>
       <c r="F32" s="9"/>
       <c r="G32" s="16" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="H32" s="9">
         <v>30</v>
@@ -3456,7 +3473,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="17" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>20</v>
@@ -3466,10 +3483,10 @@
       </c>
       <c r="M32" s="8"/>
       <c r="N32" s="8" t="s">
-        <v>120</v>
+        <v>23</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="P32" s="9" t="s">
         <v>19</v>
@@ -3484,7 +3501,7 @@
         <v>130</v>
       </c>
       <c r="T32" s="12" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="U32" s="10" t="s">
         <v>131</v>
@@ -3501,41 +3518,53 @@
         <v>138</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>10</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="E33" s="13"/>
       <c r="F33" s="9"/>
       <c r="G33" s="16" t="s">
-        <v>10</v>
+        <v>268</v>
       </c>
       <c r="H33" s="9">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>133</v>
+        <v>269</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="9"/>
+      <c r="N33" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="O33" s="9" t="s">
+        <v>281</v>
+      </c>
       <c r="P33" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="12"/>
-      <c r="U33" s="10"/>
+      <c r="Q33" s="10">
+        <v>6</v>
+      </c>
+      <c r="R33" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="S33" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="T33" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="U33" s="10" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
@@ -3551,52 +3580,38 @@
         <v>125</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>126</v>
+        <v>10</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="16" t="s">
-        <v>126</v>
+        <v>10</v>
       </c>
       <c r="H34" s="9">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="30" t="s">
-        <v>134</v>
+      <c r="J34" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M34" s="8"/>
-      <c r="N34" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O34" s="27" t="s">
-        <v>128</v>
-      </c>
+      <c r="N34" s="8"/>
+      <c r="O34" s="9"/>
       <c r="P34" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q34" s="10">
-        <v>6</v>
-      </c>
-      <c r="R34" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="S34" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="T34" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="U34" s="10" t="s">
-        <v>131</v>
-      </c>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="12"/>
+      <c r="U34" s="10"/>
     </row>
     <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
@@ -3609,21 +3624,23 @@
         <v>138</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E35" s="13"/>
+        <v>125</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>126</v>
+      </c>
       <c r="F35" s="9"/>
       <c r="G35" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H35" s="9">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J35" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
@@ -3633,13 +3650,13 @@
       </c>
       <c r="M35" s="8"/>
       <c r="N35" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="O35" s="28" t="s">
-        <v>136</v>
+        <v>32</v>
+      </c>
+      <c r="O35" s="27" t="s">
+        <v>128</v>
       </c>
       <c r="P35" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q35" s="10">
         <v>6</v>
@@ -3651,34 +3668,70 @@
         <v>130</v>
       </c>
       <c r="T35" s="12" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="U35" s="10" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="15"/>
+      <c r="A36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>127</v>
+      </c>
       <c r="E36" s="13"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="6"/>
+      <c r="G36" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H36" s="9">
+        <v>34</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J36" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="10"/>
-      <c r="T36" s="12"/>
-      <c r="U36" s="10"/>
+      <c r="N36" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O36" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="P36" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q36" s="10">
+        <v>6</v>
+      </c>
+      <c r="R36" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="S36" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="T36" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="U36" s="10" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
@@ -4508,6 +4561,29 @@
       <c r="T72" s="12"/>
       <c r="U72" s="10"/>
     </row>
+    <row r="73" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="17"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="8"/>
+      <c r="N73" s="8"/>
+      <c r="O73" s="9"/>
+      <c r="P73" s="9"/>
+      <c r="Q73" s="10"/>
+      <c r="R73" s="11"/>
+      <c r="S73" s="10"/>
+      <c r="T73" s="12"/>
+      <c r="U73" s="10"/>
+    </row>
     <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4521,192 +4597,192 @@
     <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>92</v>
-      </c>
-    </row>
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
     </row>
     <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
     </row>
     <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4874,12 +4950,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4894,41 +4964,77 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N72</xm:sqref>
+          <xm:sqref>N3:N20 N22:N73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A72</xm:sqref>
+          <xm:sqref>A3:A20 A22:A73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I72 K3:K72 P3:P72</xm:sqref>
+          <xm:sqref>K22:K73 I22:I73 I3:I20 K3:K20 P3:P20 P22:P73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L72</xm:sqref>
+          <xm:sqref>L3:L20 L22:L73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M72</xm:sqref>
+          <xm:sqref>M3:M20 M22:M73</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]DATOS!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>M21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]DATOS!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>L21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]DATOS!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>P21 K21 I21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]DATOS!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>A21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]DATOS!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>N21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Cambios en ícono de recurso
Se adicionaron íconos de recurso
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion08/ESCALETA_LE_06_08_CO_VERSION2.xlsx
+++ b/fuentes/contenidos/grado06/guion08/ESCALETA_LE_06_08_CO_VERSION2.xlsx
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -863,9 +862,6 @@
     <t>Refuerza tu aprendizaje: Informar y opinar</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: respetar la opinión</t>
-  </si>
-  <si>
     <t>Actividad de reflexión sobre las actitudes al opinar</t>
   </si>
   <si>
@@ -915,6 +911,9 @@
   </si>
   <si>
     <t>Recurso M10A-03</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Reconoce opiniones</t>
   </si>
 </sst>
 </file>
@@ -967,7 +966,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1043,6 +1042,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1143,7 +1148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1201,16 +1206,34 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1258,24 +1281,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1584,7 +1590,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,101 +1619,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="K1" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="47"/>
-      <c r="O1" s="35" t="s">
+      <c r="N1" s="53"/>
+      <c r="O1" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="R1" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="54" t="s">
+      <c r="T1" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="U1" s="35" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="42"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="48"/>
       <c r="M2" s="26" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="53"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="36"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C3" s="31" t="s">
         <v>138</v>
@@ -1766,7 +1772,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C4" s="31" t="s">
         <v>138</v>
@@ -1825,7 +1831,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>138</v>
@@ -1884,7 +1890,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>138</v>
@@ -1943,7 +1949,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>138</v>
@@ -2002,7 +2008,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C8" s="31" t="s">
         <v>138</v>
@@ -2061,7 +2067,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C9" s="31" t="s">
         <v>138</v>
@@ -2118,7 +2124,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C10" s="31" t="s">
         <v>138</v>
@@ -2153,7 +2159,7 @@
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P10" s="9" t="s">
         <v>19</v>
@@ -2179,7 +2185,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>138</v>
@@ -2242,7 +2248,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>138</v>
@@ -2279,7 +2285,7 @@
         <v>36</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="P12" s="9" t="s">
         <v>19</v>
@@ -2305,7 +2311,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C13" s="31" t="s">
         <v>138</v>
@@ -2368,7 +2374,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C14" s="31" t="s">
         <v>138</v>
@@ -2429,7 +2435,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>138</v>
@@ -2490,7 +2496,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C16" s="31" t="s">
         <v>138</v>
@@ -2523,7 +2529,7 @@
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P16" s="9" t="s">
         <v>19</v>
@@ -2549,7 +2555,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>138</v>
@@ -2582,7 +2588,7 @@
         <v>23</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P17" s="9" t="s">
         <v>19</v>
@@ -2608,7 +2614,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C18" s="31" t="s">
         <v>138</v>
@@ -2669,7 +2675,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C19" s="31" t="s">
         <v>138</v>
@@ -2730,7 +2736,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C20" s="31" t="s">
         <v>138</v>
@@ -2791,7 +2797,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>138</v>
@@ -2800,11 +2806,11 @@
         <v>142</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H21" s="9">
         <v>19</v>
@@ -2813,7 +2819,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>20</v>
@@ -2826,7 +2832,7 @@
         <v>43</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P21" s="9" t="s">
         <v>19</v>
@@ -2841,7 +2847,7 @@
         <v>130</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="U21" s="10" t="s">
         <v>131</v>
@@ -2852,7 +2858,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C22" s="31" t="s">
         <v>138</v>
@@ -2885,7 +2891,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
       <c r="O22" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P22" s="9" t="s">
         <v>19</v>
@@ -2911,7 +2917,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C23" s="31" t="s">
         <v>138</v>
@@ -2972,7 +2978,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C24" s="31" t="s">
         <v>138</v>
@@ -3031,7 +3037,7 @@
         <v>16</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C25" s="31" t="s">
         <v>138</v>
@@ -3092,7 +3098,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C26" s="31" t="s">
         <v>138</v>
@@ -3153,7 +3159,7 @@
         <v>16</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C27" s="31" t="s">
         <v>138</v>
@@ -3188,7 +3194,7 @@
       </c>
       <c r="N27" s="8"/>
       <c r="O27" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P27" s="9" t="s">
         <v>19</v>
@@ -3214,7 +3220,7 @@
         <v>16</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C28" s="31" t="s">
         <v>138</v>
@@ -3275,7 +3281,7 @@
         <v>16</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C29" s="31" t="s">
         <v>138</v>
@@ -3287,8 +3293,8 @@
         <v>122</v>
       </c>
       <c r="F29" s="9"/>
-      <c r="G29" s="16" t="s">
-        <v>271</v>
+      <c r="G29" s="58" t="s">
+        <v>288</v>
       </c>
       <c r="H29" s="9">
         <v>27</v>
@@ -3297,7 +3303,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K29" s="7" t="s">
         <v>20</v>
@@ -3310,7 +3316,7 @@
         <v>36</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P29" s="9" t="s">
         <v>20</v>
@@ -3325,7 +3331,7 @@
         <v>130</v>
       </c>
       <c r="T29" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="U29" s="10" t="s">
         <v>131</v>
@@ -3336,7 +3342,7 @@
         <v>16</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C30" s="31" t="s">
         <v>138</v>
@@ -3395,7 +3401,7 @@
         <v>16</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C31" s="31" t="s">
         <v>138</v>
@@ -3454,7 +3460,7 @@
         <v>16</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C32" s="31" t="s">
         <v>138</v>
@@ -3513,7 +3519,7 @@
         <v>16</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C33" s="31" t="s">
         <v>138</v>
@@ -3546,7 +3552,7 @@
         <v>120</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P33" s="9" t="s">
         <v>19</v>
@@ -3561,7 +3567,7 @@
         <v>130</v>
       </c>
       <c r="T33" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="U33" s="10" t="s">
         <v>131</v>
@@ -3572,7 +3578,7 @@
         <v>16</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C34" s="31" t="s">
         <v>138</v>
@@ -3619,7 +3625,7 @@
         <v>16</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C35" s="31" t="s">
         <v>138</v>
@@ -3680,7 +3686,7 @@
         <v>16</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C36" s="31" t="s">
         <v>138</v>
@@ -4951,12 +4957,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4971,6 +4971,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>